<commit_message>
add repair total day
</commit_message>
<xml_diff>
--- a/public/tmp/pivotsend.xlsx
+++ b/public/tmp/pivotsend.xlsx
@@ -47,40 +47,40 @@
     <t>อิ่นๆ</t>
   </si>
   <si>
-    <t>January/2023</t>
-  </si>
-  <si>
-    <t>February/2023</t>
-  </si>
-  <si>
-    <t>March/2023</t>
-  </si>
-  <si>
-    <t>April/2023</t>
-  </si>
-  <si>
-    <t>May/2023</t>
-  </si>
-  <si>
-    <t>June/2023</t>
-  </si>
-  <si>
-    <t>July/2023</t>
-  </si>
-  <si>
-    <t>August/2023</t>
-  </si>
-  <si>
-    <t>September/2023</t>
-  </si>
-  <si>
-    <t>October/2023</t>
-  </si>
-  <si>
-    <t>November/2023</t>
-  </si>
-  <si>
-    <t>December/2023</t>
+    <t>January/2024</t>
+  </si>
+  <si>
+    <t>February/2024</t>
+  </si>
+  <si>
+    <t>March/2024</t>
+  </si>
+  <si>
+    <t>April/2024</t>
+  </si>
+  <si>
+    <t>May/2024</t>
+  </si>
+  <si>
+    <t>June/2024</t>
+  </si>
+  <si>
+    <t>July/2024</t>
+  </si>
+  <si>
+    <t>August/2024</t>
+  </si>
+  <si>
+    <t>September/2024</t>
+  </si>
+  <si>
+    <t>October/2024</t>
+  </si>
+  <si>
+    <t>November/2024</t>
+  </si>
+  <si>
+    <t>December/2024</t>
   </si>
 </sst>
 </file>
@@ -516,16 +516,16 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>544766.02</v>
+        <v>524104.8</v>
       </c>
       <c r="C2" s="2">
-        <v>440165.25</v>
+        <v>876048.93</v>
       </c>
       <c r="D2" s="2">
-        <v>975241.27</v>
+        <v>1399273.63</v>
       </c>
       <c r="E2" s="2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -548,16 +548,16 @@
         <v>11</v>
       </c>
       <c r="B3" s="2">
-        <v>781905.78</v>
+        <v>652354.35</v>
       </c>
       <c r="C3" s="2">
-        <v>851955.44</v>
+        <v>736674.67</v>
       </c>
       <c r="D3" s="2">
-        <v>1634057.48</v>
+        <v>1389029.02</v>
       </c>
       <c r="E3" s="2">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -580,16 +580,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>1029977.94</v>
+        <v>747151.45</v>
       </c>
       <c r="C4" s="2">
-        <v>1286406.05</v>
+        <v>514086.66</v>
       </c>
       <c r="D4" s="2">
-        <v>2316383.99</v>
+        <v>1257803.11</v>
       </c>
       <c r="E4" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -612,16 +612,16 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>503242.39</v>
+        <v>737993.67</v>
       </c>
       <c r="C5" s="2">
-        <v>591737.29</v>
+        <v>557027.51</v>
       </c>
       <c r="D5" s="2">
-        <v>1094979.68</v>
+        <v>1295021.18</v>
       </c>
       <c r="E5" s="2">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -644,16 +644,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>884379.52</v>
+        <v>948036.57</v>
       </c>
       <c r="C6" s="2">
-        <v>1166937.72</v>
+        <v>815706.02</v>
       </c>
       <c r="D6" s="2">
-        <v>2051317.24</v>
+        <v>1763742.59</v>
       </c>
       <c r="E6" s="2">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -676,16 +676,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>779598.25</v>
+        <v>749996.73</v>
       </c>
       <c r="C7" s="2">
-        <v>748843.48</v>
+        <v>1024235.91</v>
       </c>
       <c r="D7" s="2">
-        <v>1528441.73</v>
+        <v>1774232.64</v>
       </c>
       <c r="E7" s="2">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -708,16 +708,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>634376.59</v>
+        <v>583517.41</v>
       </c>
       <c r="C8" s="2">
-        <v>583016.48</v>
+        <v>477364.42</v>
       </c>
       <c r="D8" s="2">
-        <v>1217393.07</v>
+        <v>1060881.83</v>
       </c>
       <c r="E8" s="2">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -740,16 +740,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>839697.62</v>
+        <v>790112.79</v>
       </c>
       <c r="C9" s="2">
-        <v>870263.97</v>
+        <v>1009617.49</v>
       </c>
       <c r="D9" s="2">
-        <v>1709961.59</v>
+        <v>1799730.28</v>
       </c>
       <c r="E9" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -772,16 +772,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>613837.1</v>
+        <v>683814.54</v>
       </c>
       <c r="C10" s="2">
-        <v>580052.0</v>
+        <v>665300.69</v>
       </c>
       <c r="D10" s="2">
-        <v>1193889.1</v>
+        <v>1349115.23</v>
       </c>
       <c r="E10" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -804,16 +804,16 @@
         <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>578650.85</v>
+        <v>58959.48</v>
       </c>
       <c r="C11" s="2">
-        <v>398962.38</v>
+        <v>142860.79</v>
       </c>
       <c r="D11" s="2">
-        <v>977613.23</v>
+        <v>201820.27</v>
       </c>
       <c r="E11" s="2">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -835,65 +835,33 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2">
-        <v>723479.17</v>
-      </c>
-      <c r="C12" s="2">
-        <v>729328.55</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1452807.72</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2">
-        <v>90</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2">
-        <v>462220.49</v>
-      </c>
-      <c r="C13" s="2">
-        <v>525431.87</v>
-      </c>
-      <c r="D13" s="2">
-        <v>987652.36</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="2">
-        <v>78</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="3"/>

</xml_diff>